<commit_message>
Started to make template cells equal helper cells
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2EFDBD-98ED-4930-AC3F-88C7432B0869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834211DA-C14B-4A10-88B8-1BE35C2DD68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
     <sheet name="Sample" sheetId="3" r:id="rId2"/>
     <sheet name="Bracket" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="27">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -91,12 +104,6 @@
   </si>
   <si>
     <t>Wildcard</t>
-  </si>
-  <si>
-    <t>Wild1</t>
-  </si>
-  <si>
-    <t>Wild2</t>
   </si>
   <si>
     <t>Wildcard16</t>
@@ -471,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF535796-3E81-4006-B204-DF282F130184}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A13931-483F-4927-9D1A-B1180B1B7A69}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,14 +1297,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>6</v>
+      <c r="B1" t="str">
+        <f>Helper!D2</f>
+        <v>an1</v>
       </c>
       <c r="N1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -1306,14 +1314,15 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" t="str">
+        <f>Helper!D17</f>
+        <v>an16</v>
       </c>
       <c r="N3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>6</v>
       </c>
@@ -1322,14 +1331,15 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
+      <c r="B5" t="str">
+        <f>Helper!D9</f>
+        <v>an8</v>
       </c>
       <c r="N5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1338,14 +1348,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="B7" t="str">
+        <f>Helper!D10</f>
+        <v>an9</v>
       </c>
       <c r="N7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>6</v>
       </c>
@@ -1354,14 +1365,15 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>10</v>
+      <c r="B9" t="str">
+        <f>Helper!D6</f>
+        <v>an5</v>
       </c>
       <c r="N9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1370,14 +1382,15 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="B11" t="str">
+        <f>Helper!D13</f>
+        <v>an12</v>
       </c>
       <c r="N11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>12</v>
       </c>
@@ -1386,14 +1399,15 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>12</v>
+      <c r="B13" t="str">
+        <f>Helper!D5</f>
+        <v>an4</v>
       </c>
       <c r="N13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -1402,14 +1416,15 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>13</v>
+      <c r="B15" t="str">
+        <f>Helper!D14</f>
+        <v>an13</v>
       </c>
       <c r="N15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>6</v>
       </c>
@@ -1418,14 +1433,15 @@
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>14</v>
+      <c r="B17" t="str">
+        <f>Helper!D7</f>
+        <v>an6</v>
       </c>
       <c r="N17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>14</v>
       </c>
@@ -1434,14 +1450,15 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>15</v>
+      <c r="B19" t="str">
+        <f>Helper!D12</f>
+        <v>an11</v>
       </c>
       <c r="N19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -1450,14 +1467,15 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>16</v>
+      <c r="B21" t="str">
+        <f>Helper!D4</f>
+        <v>an3</v>
       </c>
       <c r="N21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>16</v>
       </c>
@@ -1466,14 +1484,15 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>17</v>
+      <c r="B23" t="str">
+        <f>Helper!D15</f>
+        <v>an14</v>
       </c>
       <c r="N23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>20</v>
       </c>
@@ -1482,14 +1501,15 @@
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>18</v>
+      <c r="B25" t="str">
+        <f>Helper!D8</f>
+        <v>an7</v>
       </c>
       <c r="N25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>18</v>
       </c>
@@ -1498,14 +1518,15 @@
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>19</v>
+      <c r="B27" t="str">
+        <f>Helper!D11</f>
+        <v>an10</v>
       </c>
       <c r="N27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>20</v>
       </c>
@@ -1514,14 +1535,15 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>20</v>
+      <c r="B29" t="str">
+        <f>Helper!D3</f>
+        <v>an2</v>
       </c>
       <c r="N29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>20</v>
       </c>
@@ -1530,35 +1552,38 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>21</v>
+      <c r="B31" t="str">
+        <f>Helper!D16</f>
+        <v>an15</v>
       </c>
       <c r="N31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" t="s">
         <v>26</v>
       </c>
-      <c r="H32" t="s">
-        <v>28</v>
-      </c>
       <c r="I32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>6</v>
+      <c r="B33" t="str">
+        <f>Helper!D18</f>
+        <v>an1</v>
       </c>
       <c r="N33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>Helper!A2</f>
+        <v>wild1</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1569,15 +1594,16 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>24</v>
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>Helper!A3</f>
+        <v>wild2</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1587,14 +1613,15 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>8</v>
+      <c r="B37" t="str">
+        <f>Helper!D25</f>
+        <v>an8</v>
       </c>
       <c r="N37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>8</v>
       </c>
@@ -1603,14 +1630,15 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>9</v>
+      <c r="B39" t="str">
+        <f>Helper!D26</f>
+        <v>an9</v>
       </c>
       <c r="N39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>6</v>
       </c>
@@ -1619,14 +1647,15 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>10</v>
+      <c r="B41" t="str">
+        <f>Helper!D22</f>
+        <v>an5</v>
       </c>
       <c r="N41" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>10</v>
       </c>
@@ -1635,14 +1664,15 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>11</v>
+      <c r="B43" t="str">
+        <f>Helper!D29</f>
+        <v>an12</v>
       </c>
       <c r="N43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>12</v>
       </c>
@@ -1651,14 +1681,15 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>12</v>
+      <c r="B45" t="str">
+        <f>Helper!D21</f>
+        <v>an4</v>
       </c>
       <c r="N45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>12</v>
       </c>
@@ -1667,14 +1698,15 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>13</v>
+      <c r="B47" t="str">
+        <f>Helper!D30</f>
+        <v>an13</v>
       </c>
       <c r="N47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>6</v>
       </c>
@@ -1683,14 +1715,15 @@
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>14</v>
+      <c r="B49" t="str">
+        <f>Helper!D23</f>
+        <v>an6</v>
       </c>
       <c r="N49" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>14</v>
       </c>
@@ -1699,14 +1732,15 @@
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>15</v>
+      <c r="B51" t="str">
+        <f>Helper!D28</f>
+        <v>an11</v>
       </c>
       <c r="N51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>16</v>
       </c>
@@ -1715,14 +1749,15 @@
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>16</v>
+      <c r="B53" t="str">
+        <f>Helper!D20</f>
+        <v>an3</v>
       </c>
       <c r="N53" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>16</v>
       </c>
@@ -1731,14 +1766,15 @@
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>17</v>
+      <c r="B55" t="str">
+        <f>Helper!D31</f>
+        <v>an14</v>
       </c>
       <c r="N55" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>20</v>
       </c>
@@ -1747,14 +1783,15 @@
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>18</v>
+      <c r="B57" t="str">
+        <f>Helper!D24</f>
+        <v>an7</v>
       </c>
       <c r="N57" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>18</v>
       </c>
@@ -1763,14 +1800,15 @@
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>19</v>
+      <c r="B59" t="str">
+        <f>Helper!D27</f>
+        <v>an10</v>
       </c>
       <c r="N59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>20</v>
       </c>
@@ -1779,14 +1817,15 @@
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>20</v>
+      <c r="B61" t="str">
+        <f>Helper!D19</f>
+        <v>an2</v>
       </c>
       <c r="N61" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>20</v>
       </c>
@@ -1795,8 +1834,9 @@
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>21</v>
+      <c r="B63" t="str">
+        <f>Helper!D32</f>
+        <v>an15</v>
       </c>
       <c r="N63" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Started to write to file
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAECA231-FD0D-46AC-8DC2-BBAB2F994D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F030644A-F04E-48E1-81BE-09D0B96D87B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="16">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>an2</t>
-  </si>
-  <si>
-    <t>Wildcard</t>
   </si>
   <si>
     <t>Wildcard16</t>
@@ -791,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF535796-3E81-4006-B204-DF282F130184}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,21 +1233,22 @@
       <c r="C33" s="1">
         <v>16</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>12</v>
+      <c r="D33" s="1" t="str">
+        <f>A2</f>
+        <v>Bumblebee Bat</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f>[1]Sheet1!C51</f>
-        <v>Golden Eagle</v>
+        <f>A3</f>
+        <v>Shrew Mole</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,11 +1257,11 @@
         <v>3</v>
       </c>
       <c r="C35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f>[1]Sheet1!C52</f>
-        <v>Cathedral Termite</v>
+        <f>[1]Sheet1!C51</f>
+        <v>Golden Eagle</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,11 +1270,11 @@
         <v>3</v>
       </c>
       <c r="C36" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f>[1]Sheet1!C53</f>
-        <v>Homo habilis</v>
+        <f>[1]Sheet1!C52</f>
+        <v>Cathedral Termite</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,11 +1283,11 @@
         <v>3</v>
       </c>
       <c r="C37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f>[1]Sheet1!C54</f>
-        <v>Lungfish</v>
+        <f>[1]Sheet1!C53</f>
+        <v>Homo habilis</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,11 +1296,11 @@
         <v>3</v>
       </c>
       <c r="C38" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1" t="str">
-        <f>[1]Sheet1!C55</f>
-        <v>Palaeocastor</v>
+        <f>[1]Sheet1!C54</f>
+        <v>Lungfish</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,11 +1309,11 @@
         <v>3</v>
       </c>
       <c r="C39" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="1" t="str">
-        <f>[1]Sheet1!C56</f>
-        <v>Goanna</v>
+        <f>[1]Sheet1!C55</f>
+        <v>Palaeocastor</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1324,11 +1322,11 @@
         <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f>[1]Sheet1!C57</f>
-        <v>Montezuma Oropendola</v>
+        <f>[1]Sheet1!C56</f>
+        <v>Goanna</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,11 +1335,11 @@
         <v>3</v>
       </c>
       <c r="C41" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="str">
-        <f>[1]Sheet1!C58</f>
-        <v>Veined Octopus</v>
+        <f>[1]Sheet1!C57</f>
+        <v>Montezuma Oropendola</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,11 +1348,11 @@
         <v>3</v>
       </c>
       <c r="C42" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1" t="str">
-        <f>[1]Sheet1!C59</f>
-        <v>Puffer Fish</v>
+        <f>[1]Sheet1!C58</f>
+        <v>Veined Octopus</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1363,11 +1361,11 @@
         <v>3</v>
       </c>
       <c r="C43" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" s="1" t="str">
-        <f>[1]Sheet1!C60</f>
-        <v>New Caledonian Crow</v>
+        <f>[1]Sheet1!C59</f>
+        <v>Puffer Fish</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1376,11 +1374,11 @@
         <v>3</v>
       </c>
       <c r="C44" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="str">
-        <f>[1]Sheet1!C61</f>
-        <v>Rufous Hornero</v>
+        <f>[1]Sheet1!C60</f>
+        <v>New Caledonian Crow</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,11 +1387,11 @@
         <v>3</v>
       </c>
       <c r="C45" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45" s="1" t="str">
-        <f>[1]Sheet1!C62</f>
-        <v>Trapdoor Spider</v>
+        <f>[1]Sheet1!C61</f>
+        <v>Rufous Hornero</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,11 +1400,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f>[1]Sheet1!C63</f>
-        <v>Tent-making Bat</v>
+        <f>[1]Sheet1!C62</f>
+        <v>Trapdoor Spider</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1415,11 +1413,11 @@
         <v>3</v>
       </c>
       <c r="C47" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D47" s="1" t="str">
-        <f>[1]Sheet1!C64</f>
-        <v>Bee</v>
+        <f>[1]Sheet1!C63</f>
+        <v>Tent-making Bat</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,11 +1426,11 @@
         <v>3</v>
       </c>
       <c r="C48" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f>[1]Sheet1!C65</f>
-        <v>Dung Beetle</v>
+        <f>[1]Sheet1!C64</f>
+        <v>Bee</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1441,24 +1439,24 @@
         <v>3</v>
       </c>
       <c r="C49" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f>[1]Sheet1!C66</f>
-        <v>Spongilla Fly</v>
+        <f>[1]Sheet1!C65</f>
+        <v>Dung Beetle</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f>[1]Sheet1!C35</f>
-        <v>Emperor Penguin</v>
+        <f>[1]Sheet1!C66</f>
+        <v>Spongilla Fly</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,11 +1465,11 @@
         <v>4</v>
       </c>
       <c r="C51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="str">
-        <f>[1]Sheet1!C36</f>
-        <v>Greater Rhea</v>
+        <f>[1]Sheet1!C35</f>
+        <v>Emperor Penguin</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,11 +1478,11 @@
         <v>4</v>
       </c>
       <c r="C52" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D52" s="1" t="str">
-        <f>[1]Sheet1!C37</f>
-        <v>Wolverine</v>
+        <f>[1]Sheet1!C36</f>
+        <v>Greater Rhea</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,11 +1491,11 @@
         <v>4</v>
       </c>
       <c r="C53" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53" s="1" t="str">
-        <f>[1]Sheet1!C38</f>
-        <v>Siamang</v>
+        <f>[1]Sheet1!C37</f>
+        <v>Wolverine</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,11 +1504,11 @@
         <v>4</v>
       </c>
       <c r="C54" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D54" s="1" t="str">
-        <f>[1]Sheet1!C39</f>
-        <v>Pacific Spiny Lumpsucker</v>
+        <f>[1]Sheet1!C38</f>
+        <v>Siamang</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,11 +1517,11 @@
         <v>4</v>
       </c>
       <c r="C55" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" s="1" t="str">
-        <f>[1]Sheet1!C40</f>
-        <v>Bat-Eared Fox</v>
+        <f>[1]Sheet1!C39</f>
+        <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,11 +1530,11 @@
         <v>4</v>
       </c>
       <c r="C56" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" s="1" t="str">
-        <f>[1]Sheet1!C41</f>
-        <v>Greater Flamingo</v>
+        <f>[1]Sheet1!C40</f>
+        <v>Bat-Eared Fox</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,11 +1543,11 @@
         <v>4</v>
       </c>
       <c r="C57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" s="1" t="str">
-        <f>[1]Sheet1!C42</f>
-        <v>Owl Monkey</v>
+        <f>[1]Sheet1!C41</f>
+        <v>Greater Flamingo</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1558,11 +1556,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" s="1" t="str">
-        <f>[1]Sheet1!C43</f>
-        <v>Caspian Terns</v>
+        <f>[1]Sheet1!C42</f>
+        <v>Owl Monkey</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,11 +1569,11 @@
         <v>4</v>
       </c>
       <c r="C59" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D59" s="1" t="str">
-        <f>[1]Sheet1!C44</f>
-        <v>Dyak Fruit Bat</v>
+        <f>[1]Sheet1!C43</f>
+        <v>Caspian Terns</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,11 +1582,11 @@
         <v>4</v>
       </c>
       <c r="C60" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" s="1" t="str">
-        <f>[1]Sheet1!C45</f>
-        <v>Spotted sandpiper</v>
+        <f>[1]Sheet1!C44</f>
+        <v>Dyak Fruit Bat</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1597,11 +1595,11 @@
         <v>4</v>
       </c>
       <c r="C61" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61" s="1" t="str">
-        <f>[1]Sheet1!C46</f>
-        <v>Peacock Wrasse</v>
+        <f>[1]Sheet1!C45</f>
+        <v>Spotted sandpiper</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1610,11 +1608,11 @@
         <v>4</v>
       </c>
       <c r="C62" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62" s="1" t="str">
-        <f>[1]Sheet1!C47</f>
-        <v>Darwin's Frogs</v>
+        <f>[1]Sheet1!C46</f>
+        <v>Peacock Wrasse</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1623,11 +1621,11 @@
         <v>4</v>
       </c>
       <c r="C63" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D63" s="1" t="str">
-        <f>[1]Sheet1!C48</f>
-        <v>Giant Water Bug</v>
+        <f>[1]Sheet1!C47</f>
+        <v>Darwin's Frogs</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1636,11 +1634,11 @@
         <v>4</v>
       </c>
       <c r="C64" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D64" s="1" t="str">
-        <f>[1]Sheet1!C49</f>
-        <v xml:space="preserve">Three-Spined stickleback </v>
+        <f>[1]Sheet1!C48</f>
+        <v>Giant Water Bug</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,9 +1647,22 @@
         <v>4</v>
       </c>
       <c r="C65" s="1">
+        <v>15</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f>[1]Sheet1!C49</f>
+        <v xml:space="preserve">Three-Spined stickleback </v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1">
+        <v>4</v>
+      </c>
+      <c r="C66" s="1">
         <v>16</v>
       </c>
-      <c r="D65" s="1" t="str">
+      <c r="D66" s="1" t="str">
         <f>[1]Sheet1!C50</f>
         <v>Lined Seahorse</v>
       </c>
@@ -1666,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A13931-483F-4927-9D1A-B1180B1B7A69}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,7 +1697,7 @@
         <v>Okapi</v>
       </c>
       <c r="O1" t="str">
-        <f>Helper!D34</f>
+        <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
@@ -1710,7 +1721,7 @@
         <v>Four-Striped Grass Mouse</v>
       </c>
       <c r="O3" t="str">
-        <f>Helper!D49</f>
+        <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
@@ -1734,7 +1745,7 @@
         <v>Striped Polecat</v>
       </c>
       <c r="O5" t="str">
-        <f>Helper!D41</f>
+        <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
@@ -1758,7 +1769,7 @@
         <v>Giant striped mongoose</v>
       </c>
       <c r="O7" t="str">
-        <f>Helper!D42</f>
+        <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
@@ -1782,7 +1793,7 @@
         <v>Side-striped jackal</v>
       </c>
       <c r="O9" t="str">
-        <f>Helper!D38</f>
+        <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
@@ -1806,7 +1817,7 @@
         <v>Striped Possum</v>
       </c>
       <c r="O11" t="str">
-        <f>Helper!D45</f>
+        <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
@@ -1830,7 +1841,7 @@
         <v>Striped dolphin</v>
       </c>
       <c r="O13" t="str">
-        <f>Helper!D37</f>
+        <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
@@ -1854,7 +1865,7 @@
         <v>Chequered elephant shrew</v>
       </c>
       <c r="O15" t="str">
-        <f>Helper!D46</f>
+        <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
@@ -1878,7 +1889,7 @@
         <v>Wildcat</v>
       </c>
       <c r="O17" t="str">
-        <f>Helper!D39</f>
+        <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
@@ -1902,7 +1913,7 @@
         <v>Highland Streaked Tenrec</v>
       </c>
       <c r="O19" t="str">
-        <f>Helper!D44</f>
+        <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
@@ -1926,7 +1937,7 @@
         <v>Striped hyena</v>
       </c>
       <c r="O21" t="str">
-        <f>Helper!D36</f>
+        <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
@@ -1950,7 +1961,7 @@
         <v>Fire-footed Rope Squirrel</v>
       </c>
       <c r="O23" t="str">
-        <f>Helper!D47</f>
+        <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
@@ -1974,7 +1985,7 @@
         <v>Striped Rabbit</v>
       </c>
       <c r="O25" t="str">
-        <f>Helper!D40</f>
+        <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
@@ -1998,7 +2009,7 @@
         <v>Numbat</v>
       </c>
       <c r="O27" t="str">
-        <f>Helper!D43</f>
+        <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
@@ -2022,7 +2033,7 @@
         <v>Kudu</v>
       </c>
       <c r="O29" t="str">
-        <f>Helper!D35</f>
+        <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
@@ -2046,7 +2057,7 @@
         <v>Badger Bat</v>
       </c>
       <c r="O31" t="str">
-        <f>Helper!D48</f>
+        <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
@@ -2055,13 +2066,13 @@
         <v>32</v>
       </c>
       <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" t="s">
         <v>14</v>
-      </c>
-      <c r="I32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2073,7 +2084,7 @@
         <v>Sea Otter</v>
       </c>
       <c r="O33" t="str">
-        <f>Helper!D50</f>
+        <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
@@ -2097,10 +2108,10 @@
         <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O35" t="str">
-        <f>Helper!D65</f>
+        <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
@@ -2128,7 +2139,7 @@
         <v>Southern Ningaui</v>
       </c>
       <c r="O37" t="str">
-        <f>Helper!D57</f>
+        <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
@@ -2152,7 +2163,7 @@
         <v>Grasshopper Mouse</v>
       </c>
       <c r="O39" t="str">
-        <f>Helper!D58</f>
+        <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
@@ -2176,7 +2187,7 @@
         <v>Sibree Dwarf Lemur</v>
       </c>
       <c r="O41" t="str">
-        <f>Helper!D54</f>
+        <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
@@ -2200,7 +2211,7 @@
         <v>Silver Pika</v>
       </c>
       <c r="O43" t="str">
-        <f>Helper!D61</f>
+        <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
@@ -2224,7 +2235,7 @@
         <v>Mara</v>
       </c>
       <c r="O45" t="str">
-        <f>Helper!D53</f>
+        <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
@@ -2248,7 +2259,7 @@
         <v>Siberian Chipmunk</v>
       </c>
       <c r="O47" t="str">
-        <f>Helper!D62</f>
+        <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
@@ -2272,7 +2283,7 @@
         <v>Itjaritjari</v>
       </c>
       <c r="O49" t="str">
-        <f>Helper!D55</f>
+        <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
@@ -2296,7 +2307,7 @@
         <v>Silky Anteater</v>
       </c>
       <c r="O51" t="str">
-        <f>Helper!D60</f>
+        <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
@@ -2320,7 +2331,7 @@
         <v>Dik Dik</v>
       </c>
       <c r="O53" t="str">
-        <f>Helper!D52</f>
+        <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
@@ -2344,7 +2355,7 @@
         <v>Colo Colo Opossum</v>
       </c>
       <c r="O55" t="str">
-        <f>Helper!D63</f>
+        <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
@@ -2368,7 +2379,7 @@
         <v>Bulldog Bat</v>
       </c>
       <c r="O57" t="str">
-        <f>Helper!D56</f>
+        <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
@@ -2392,7 +2403,7 @@
         <v>Thor's Hero Shrew</v>
       </c>
       <c r="O59" t="str">
-        <f>Helper!D59</f>
+        <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
@@ -2416,7 +2427,7 @@
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
       <c r="O61" t="str">
-        <f>Helper!D51</f>
+        <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
@@ -2440,7 +2451,7 @@
         <v>Pygmy Jerboa</v>
       </c>
       <c r="O63" t="str">
-        <f>Helper!D64</f>
+        <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
     </row>
@@ -2454,12 +2465,787 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD84F6-D856-4FCA-9254-65D9DBB06268}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>Helper!D2</f>
+        <v>Okapi</v>
+      </c>
+      <c r="O1" t="str">
+        <f>Helper!D35</f>
+        <v>Golden Eagle</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Helper!D17</f>
+        <v>Four-Striped Grass Mouse</v>
+      </c>
+      <c r="O3" t="str">
+        <f>Helper!D50</f>
+        <v>Spongilla Fly</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Helper!D9</f>
+        <v>Striped Polecat</v>
+      </c>
+      <c r="O5" t="str">
+        <f>Helper!D42</f>
+        <v>Veined Octopus</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Helper!D10</f>
+        <v>Giant striped mongoose</v>
+      </c>
+      <c r="O7" t="str">
+        <f>Helper!D43</f>
+        <v>Puffer Fish</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Helper!D6</f>
+        <v>Side-striped jackal</v>
+      </c>
+      <c r="O9" t="str">
+        <f>Helper!D39</f>
+        <v>Palaeocastor</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Helper!D13</f>
+        <v>Striped Possum</v>
+      </c>
+      <c r="O11" t="str">
+        <f>Helper!D46</f>
+        <v>Trapdoor Spider</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Helper!D5</f>
+        <v>Striped dolphin</v>
+      </c>
+      <c r="O13" t="str">
+        <f>Helper!D38</f>
+        <v>Lungfish</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Helper!D14</f>
+        <v>Chequered elephant shrew</v>
+      </c>
+      <c r="O15" t="str">
+        <f>Helper!D47</f>
+        <v>Tent-making Bat</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Helper!D7</f>
+        <v>Wildcat</v>
+      </c>
+      <c r="O17" t="str">
+        <f>Helper!D40</f>
+        <v>Goanna</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Helper!D12</f>
+        <v>Highland Streaked Tenrec</v>
+      </c>
+      <c r="O19" t="str">
+        <f>Helper!D45</f>
+        <v>Rufous Hornero</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Helper!D4</f>
+        <v>Striped hyena</v>
+      </c>
+      <c r="O21" t="str">
+        <f>Helper!D37</f>
+        <v>Homo habilis</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="str">
+        <f>Helper!D15</f>
+        <v>Fire-footed Rope Squirrel</v>
+      </c>
+      <c r="O23" t="str">
+        <f>Helper!D48</f>
+        <v>Bee</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="C25" t="str">
+        <f>Helper!D8</f>
+        <v>Striped Rabbit</v>
+      </c>
+      <c r="O25" t="str">
+        <f>Helper!D41</f>
+        <v>Montezuma Oropendola</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="N26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Helper!D11</f>
+        <v>Numbat</v>
+      </c>
+      <c r="O27" t="str">
+        <f>Helper!D44</f>
+        <v>New Caledonian Crow</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="C29" t="str">
+        <f>Helper!D3</f>
+        <v>Kudu</v>
+      </c>
+      <c r="O29" t="str">
+        <f>Helper!D36</f>
+        <v>Cathedral Termite</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="C31" t="str">
+        <f>Helper!D16</f>
+        <v>Badger Bat</v>
+      </c>
+      <c r="O31" t="str">
+        <f>Helper!D49</f>
+        <v>Dung Beetle</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="C33" t="str">
+        <f>Helper!D18</f>
+        <v>Sea Otter</v>
+      </c>
+      <c r="O33" t="str">
+        <f>Helper!D51</f>
+        <v>Emperor Penguin</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="str">
+        <f>Helper!A2</f>
+        <v>Bumblebee Bat</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" t="str">
+        <f>Helper!D66</f>
+        <v>Lined Seahorse</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="str">
+        <f>Helper!A3</f>
+        <v>Shrew Mole</v>
+      </c>
+      <c r="E36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="C37" t="str">
+        <f>Helper!D25</f>
+        <v>Southern Ningaui</v>
+      </c>
+      <c r="O37" t="str">
+        <f>Helper!D58</f>
+        <v>Owl Monkey</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="N38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="C39" t="str">
+        <f>Helper!D26</f>
+        <v>Grasshopper Mouse</v>
+      </c>
+      <c r="O39" t="str">
+        <f>Helper!D59</f>
+        <v>Caspian Terns</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="C41" t="str">
+        <f>Helper!D22</f>
+        <v>Sibree Dwarf Lemur</v>
+      </c>
+      <c r="O41" t="str">
+        <f>Helper!D55</f>
+        <v>Pacific Spiny Lumpsucker</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="C43" t="str">
+        <f>Helper!D29</f>
+        <v>Silver Pika</v>
+      </c>
+      <c r="O43" t="str">
+        <f>Helper!D62</f>
+        <v>Peacock Wrasse</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="M44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="C45" t="str">
+        <f>Helper!D21</f>
+        <v>Mara</v>
+      </c>
+      <c r="O45" t="str">
+        <f>Helper!D54</f>
+        <v>Siamang</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="N46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="C47" t="str">
+        <f>Helper!D30</f>
+        <v>Siberian Chipmunk</v>
+      </c>
+      <c r="O47" t="str">
+        <f>Helper!D63</f>
+        <v>Darwin's Frogs</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="G48" t="s">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="C49" t="str">
+        <f>Helper!D23</f>
+        <v>Itjaritjari</v>
+      </c>
+      <c r="O49" t="str">
+        <f>Helper!D56</f>
+        <v>Bat-Eared Fox</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="N50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="C51" t="str">
+        <f>Helper!D28</f>
+        <v>Silky Anteater</v>
+      </c>
+      <c r="O51" t="str">
+        <f>Helper!D61</f>
+        <v>Spotted sandpiper</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="M52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="C53" t="str">
+        <f>Helper!D20</f>
+        <v>Dik Dik</v>
+      </c>
+      <c r="O53" t="str">
+        <f>Helper!D53</f>
+        <v>Wolverine</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="N54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="C55" t="str">
+        <f>Helper!D31</f>
+        <v>Colo Colo Opossum</v>
+      </c>
+      <c r="O55" t="str">
+        <f>Helper!D64</f>
+        <v>Giant Water Bug</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="L56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="C57" t="str">
+        <f>Helper!D24</f>
+        <v>Bulldog Bat</v>
+      </c>
+      <c r="O57" t="str">
+        <f>Helper!D57</f>
+        <v>Greater Flamingo</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="C59" t="str">
+        <f>Helper!D27</f>
+        <v>Thor's Hero Shrew</v>
+      </c>
+      <c r="O59" t="str">
+        <f>Helper!D60</f>
+        <v>Dyak Fruit Bat</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="M60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="C61" t="str">
+        <f>Helper!D19</f>
+        <v xml:space="preserve">Rock Hyrax </v>
+      </c>
+      <c r="O61" t="str">
+        <f>Helper!D52</f>
+        <v>Greater Rhea</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="N62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="C63" t="str">
+        <f>Helper!D32</f>
+        <v>Pygmy Jerboa</v>
+      </c>
+      <c r="O63" t="str">
+        <f>Helper!D65</f>
+        <v xml:space="preserve">Three-Spined stickleback </v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correctly writes the winners of the first round of the first bracket.
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F030644A-F04E-48E1-81BE-09D0B96D87B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FF09C-AAE0-49F0-ABDB-5DAC9DCC4A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1215" windowWidth="28800" windowHeight="14385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
     <sheet name="Sample" sheetId="3" r:id="rId2"/>
     <sheet name="Bracket" sheetId="4" r:id="rId3"/>
+    <sheet name="Bracket1" r:id="rId9" sheetId="5"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="26">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -87,11 +88,42 @@
   <si>
     <t>Champ</t>
   </si>
+  <si>
+    <t>Okapi</t>
+  </si>
+  <si>
+    <t>Giant striped mongoose</t>
+  </si>
+  <si>
+    <t>Side-striped jackal</t>
+  </si>
+  <si>
+    <t>Striped dolphin</t>
+  </si>
+  <si>
+    <t>Wildcat</t>
+  </si>
+  <si>
+    <t>Striped hyena</t>
+  </si>
+  <si>
+    <t>Striped Rabbit</t>
+  </si>
+  <si>
+    <t>Kudu</t>
+  </si>
+  <si>
+    <t>Striped Polecat</t>
+  </si>
+  <si>
+    <t>Numbat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,16 +822,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF535796-3E81-4006-B204-DF282F130184}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="36.140625"/>
+    <col min="2" max="2" customWidth="true" width="41.28515625"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125"/>
+    <col min="4" max="4" customWidth="true" width="25.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,774 +1715,774 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="25.42578125"/>
+    <col min="15" max="15" customWidth="true" width="23.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="D2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="A4" s="0">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>5</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>7</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="F8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>9</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>11</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str">
+      <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>13</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>15</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str">
+      <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>16</v>
       </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>17</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str">
+      <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>19</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>21</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str">
+      <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>22</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>23</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>25</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str">
+      <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>27</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str">
+      <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>28</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>29</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str">
+      <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>30</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>31</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str">
+      <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>32</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>33</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str">
+      <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>34</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="D34" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O35" t="str">
+      <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>36</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s">
-        <v>4</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="E36" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>37</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str">
+      <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>39</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str">
+      <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>40</v>
       </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="F40" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>41</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str">
+      <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>42</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>43</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str">
+      <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>44</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>45</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str">
+      <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>46</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>47</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str">
+      <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>48</v>
       </c>
-      <c r="G48" t="s">
-        <v>4</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="G48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>49</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str">
+      <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>50</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>51</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str">
+      <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="0">
         <v>52</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="0">
         <v>53</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str">
+      <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="0">
         <v>54</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="0">
         <v>55</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str">
+      <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="0">
         <v>56</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="0">
         <v>57</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str">
+      <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="0">
         <v>58</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="0">
         <v>59</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str">
+      <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="0">
         <v>60</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="0">
         <v>61</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str">
+      <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="0">
         <v>62</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="0">
         <v>63</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str">
+      <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
@@ -2467,780 +2499,732 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD84F6-D856-4FCA-9254-65D9DBB06268}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.7109375"/>
+    <col min="3" max="3" customWidth="true" width="25.42578125"/>
+    <col min="15" max="15" customWidth="true" width="23.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" t="str" s="0">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str">
+      <c r="O1" t="str" s="0">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="D2" t="s" s="0">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" t="str" s="0">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str">
+      <c r="O3" t="str" s="0">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="A4" s="0">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>5</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" t="str" s="0">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" t="str" s="0">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
-        <v>5</v>
+    <row r="6">
+      <c r="D6" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>7</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" t="str" s="0">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str">
+      <c r="O7" t="str" s="0">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="F8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>9</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" t="str" s="0">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str">
+      <c r="O9" t="str" s="0">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="N10" t="s">
-        <v>6</v>
+    <row r="10">
+      <c r="D10" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>11</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" t="str" s="0">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str">
+      <c r="O11" t="str" s="0">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>13</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" t="str" s="0">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13" t="str" s="0">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="N14" t="s">
-        <v>7</v>
+    <row r="14">
+      <c r="D14" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>15</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" t="str" s="0">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str">
+      <c r="O15" t="str" s="0">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>16</v>
       </c>
-      <c r="G16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="G16" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>17</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" t="str" s="0">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str">
+      <c r="O17" t="str" s="0">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="N18" t="s">
-        <v>8</v>
+    <row r="18">
+      <c r="D18" t="s" s="0">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>19</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" t="str" s="0">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O19" t="str" s="0">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>21</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" t="str" s="0">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str">
+      <c r="O21" t="str" s="0">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="N22" t="s">
-        <v>9</v>
+    <row r="22">
+      <c r="D22" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>23</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" t="str" s="0">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23" t="str" s="0">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>25</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" t="str" s="0">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str">
+      <c r="O25" t="str" s="0">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="N26" t="s">
-        <v>10</v>
+    <row r="26">
+      <c r="D26" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>27</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" t="str" s="0">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str">
+      <c r="O27" t="str" s="0">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>28</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>29</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" t="str" s="0">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str">
+      <c r="O29" t="str" s="0">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="N30" t="s">
-        <v>11</v>
+    <row r="30">
+      <c r="D30" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>31</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" t="str" s="0">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str">
+      <c r="O31" t="str" s="0">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>32</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>33</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" t="str" s="0">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str">
+      <c r="O33" t="str" s="0">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>34</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" t="str" s="0">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s">
-        <v>4</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="D34" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O35" t="str">
+      <c r="O35" t="str" s="0">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>36</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" t="str" s="0">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s">
-        <v>4</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="E36" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="0">
         <v>37</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" t="str" s="0">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str">
+      <c r="O37" t="str" s="0">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="N38" t="s">
+      <c r="N38" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>39</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" t="str" s="0">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str">
+      <c r="O39" t="str" s="0">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>40</v>
       </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="F40" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>41</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" t="str" s="0">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str">
+      <c r="O41" t="str" s="0">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>42</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="N42" t="s">
+      <c r="N42" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>43</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" t="str" s="0">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str">
+      <c r="O43" t="str" s="0">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>44</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>45</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" t="str" s="0">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str">
+      <c r="O45" t="str" s="0">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>46</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N46" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>47</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" t="str" s="0">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str">
+      <c r="O47" t="str" s="0">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>48</v>
       </c>
-      <c r="G48" t="s">
-        <v>4</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="G48" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>49</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" t="str" s="0">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str">
+      <c r="O49" t="str" s="0">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>50</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N50" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>51</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" t="str" s="0">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str">
+      <c r="O51" t="str" s="0">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="0">
         <v>52</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="0">
         <v>53</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" t="str" s="0">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str">
+      <c r="O53" t="str" s="0">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="0">
         <v>54</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="0">
         <v>55</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" t="str" s="0">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str">
+      <c r="O55" t="str" s="0">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="0">
         <v>56</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="A57" s="0">
         <v>57</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" t="str" s="0">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str">
+      <c r="O57" t="str" s="0">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="A58" s="0">
         <v>58</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="A59" s="0">
         <v>59</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" t="str" s="0">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str">
+      <c r="O59" t="str" s="0">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="A60" s="0">
         <v>60</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61">
+      <c r="A61" s="0">
         <v>61</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" t="str" s="0">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str">
+      <c r="O61" t="str" s="0">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="A62" s="0">
         <v>62</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="0">
         <v>63</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" t="str" s="0">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str">
+      <c r="O63" t="str" s="0">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
@@ -3248,4 +3232,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="D2:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="D2" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Works!!! Changed previous method so it can compare all rounds except wildcard and championship. Only thing left is to make it so that it can download(?) the real bracket to create a bracket on the computer instead of having the fie be on the computer originally.
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ks4292\IdeaProjects\Mam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pants\IdeaProjects\Mam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46C7DA4-FF98-4E54-AC0B-95328EACBF6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41A5F64-F34E-438E-9AEE-62EB3A317D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1215" windowWidth="28800" windowHeight="14385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="48" windowWidth="17280" windowHeight="8928" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Helper" sheetId="2" r:id="rId1"/>
@@ -22,11 +22,24 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="55">
   <si>
     <t>Type in the two Wildcard animals below</t>
   </si>
@@ -94,128 +107,109 @@
     <t>Kudu</t>
   </si>
   <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Hyrax </t>
+  </si>
+  <si>
+    <t>Golden Eagle</t>
+  </si>
+  <si>
+    <t>Homo habilis</t>
+  </si>
+  <si>
+    <t>Cathedral Termite</t>
+  </si>
+  <si>
+    <t>Emperor Penguin</t>
+  </si>
+  <si>
+    <t>Owl Monkey</t>
+  </si>
+  <si>
+    <t>Siamang</t>
+  </si>
+  <si>
+    <t>Striped Rabbit</t>
+  </si>
+  <si>
+    <t>Shrew Mole</t>
+  </si>
+  <si>
+    <t>Greater Rhea</t>
+  </si>
+  <si>
+    <t>Montezuma Oropendola</t>
+  </si>
+  <si>
+    <t>Dik Dik</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>Giant striped mongoose</t>
+  </si>
+  <si>
+    <t>Tent-making Bat</t>
+  </si>
+  <si>
+    <t>Thor's Hero Shrew</t>
+  </si>
+  <si>
+    <t>Veined Octopus</t>
+  </si>
+  <si>
+    <t>Palaeocastor</t>
+  </si>
+  <si>
+    <t>Goanna</t>
+  </si>
+  <si>
+    <t>Grasshopper Mouse</t>
+  </si>
+  <si>
+    <t>Sibree Dwarf Lemur</t>
+  </si>
+  <si>
+    <t>Pacific Spiny Lumpsucker</t>
+  </si>
+  <si>
+    <t>Silky Anteater</t>
+  </si>
+  <si>
+    <t>Spotted sandpiper</t>
+  </si>
+  <si>
+    <t>Greater Flamingo</t>
+  </si>
+  <si>
     <t>Striped Polecat</t>
   </si>
   <si>
-    <t>Numbat</t>
-  </si>
-  <si>
-    <t>Silver Pika</t>
-  </si>
-  <si>
-    <t>Mara</t>
+    <t>New Caledonian Crow</t>
   </si>
   <si>
     <t>Sea Otter</t>
   </si>
   <si>
+    <t>Lungfish</t>
+  </si>
+  <si>
     <t>Bulldog Bat</t>
   </si>
   <si>
-    <t xml:space="preserve">Rock Hyrax </t>
-  </si>
-  <si>
-    <t>Golden Eagle</t>
-  </si>
-  <si>
-    <t>Palaeocastor</t>
-  </si>
-  <si>
-    <t>Lungfish</t>
-  </si>
-  <si>
-    <t>Homo habilis</t>
-  </si>
-  <si>
-    <t>Cathedral Termite</t>
-  </si>
-  <si>
     <t>Bumblebee Bat</t>
   </si>
   <si>
-    <t>Puffer Fish</t>
-  </si>
-  <si>
-    <t>Emperor Penguin</t>
-  </si>
-  <si>
-    <t>Southern Ningaui</t>
-  </si>
-  <si>
-    <t>Owl Monkey</t>
-  </si>
-  <si>
-    <t>Peacock Wrasse</t>
-  </si>
-  <si>
-    <t>Siamang</t>
-  </si>
-  <si>
-    <t>Bat-Eared Fox</t>
-  </si>
-  <si>
-    <t>Wolverine</t>
-  </si>
-  <si>
-    <t>Greater Flamingo</t>
-  </si>
-  <si>
-    <t>Chequered elephant shrew</t>
-  </si>
-  <si>
-    <t>Goanna</t>
-  </si>
-  <si>
-    <t>New Caledonian Crow</t>
-  </si>
-  <si>
-    <t>Silky Anteater</t>
-  </si>
-  <si>
-    <t>Striped Rabbit</t>
-  </si>
-  <si>
-    <t>Colo Colo Opossum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three-Spined stickleback </t>
-  </si>
-  <si>
-    <t>Shrew Mole</t>
-  </si>
-  <si>
-    <t>Giant striped mongoose</t>
-  </si>
-  <si>
-    <t>Veined Octopus</t>
-  </si>
-  <si>
-    <t>Highland Streaked Tenrec</t>
-  </si>
-  <si>
-    <t>Rufous Hornero</t>
-  </si>
-  <si>
-    <t>Grasshopper Mouse</t>
-  </si>
-  <si>
-    <t>Sibree Dwarf Lemur</t>
-  </si>
-  <si>
-    <t>Pacific Spiny Lumpsucker</t>
-  </si>
-  <si>
-    <t>Giant Water Bug</t>
-  </si>
-  <si>
-    <t>Greater Rhea</t>
+    <t>Dung Beetle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +268,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -915,15 +909,15 @@
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.140625"/>
-    <col min="2" max="2" customWidth="true" width="41.28515625"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125"/>
-    <col min="4" max="4" customWidth="true" width="25.0"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>[1]Sheet1!C17</f>
         <v>Bumblebee Bat</v>
@@ -953,7 +947,7 @@
         <v>Okapi</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>[1]Sheet1!C18</f>
         <v>Shrew Mole</v>
@@ -969,7 +963,7 @@
         <v>Kudu</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>1</v>
@@ -982,7 +976,7 @@
         <v>Striped hyena</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>1</v>
@@ -995,7 +989,7 @@
         <v>Striped dolphin</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>1</v>
@@ -1008,7 +1002,7 @@
         <v>Side-striped jackal</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>1</v>
@@ -1021,7 +1015,7 @@
         <v>Wildcat</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>1</v>
@@ -1034,7 +1028,7 @@
         <v>Striped Rabbit</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>1</v>
@@ -1047,7 +1041,7 @@
         <v>Striped Polecat</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>1</v>
@@ -1060,7 +1054,7 @@
         <v>Giant striped mongoose</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>1</v>
@@ -1073,7 +1067,7 @@
         <v>Numbat</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>1</v>
@@ -1086,7 +1080,7 @@
         <v>Highland Streaked Tenrec</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>1</v>
@@ -1099,7 +1093,7 @@
         <v>Striped Possum</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1">
         <v>1</v>
@@ -1112,7 +1106,7 @@
         <v>Chequered elephant shrew</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1">
         <v>1</v>
@@ -1125,7 +1119,7 @@
         <v>Fire-footed Rope Squirrel</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>1</v>
@@ -1138,7 +1132,7 @@
         <v>Badger Bat</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1">
         <v>1</v>
@@ -1151,7 +1145,7 @@
         <v>Four-Striped Grass Mouse</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -1164,7 +1158,7 @@
         <v>Sea Otter</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1">
         <v>2</v>
@@ -1177,7 +1171,7 @@
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>2</v>
@@ -1190,7 +1184,7 @@
         <v>Dik Dik</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1">
         <v>2</v>
@@ -1203,7 +1197,7 @@
         <v>Mara</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1">
         <v>2</v>
@@ -1216,7 +1210,7 @@
         <v>Sibree Dwarf Lemur</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1">
         <v>2</v>
@@ -1229,7 +1223,7 @@
         <v>Itjaritjari</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1">
         <v>2</v>
@@ -1242,7 +1236,7 @@
         <v>Bulldog Bat</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>2</v>
@@ -1255,7 +1249,7 @@
         <v>Southern Ningaui</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>2</v>
@@ -1268,7 +1262,7 @@
         <v>Grasshopper Mouse</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1">
         <v>2</v>
@@ -1281,7 +1275,7 @@
         <v>Thor's Hero Shrew</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1">
         <v>2</v>
@@ -1294,7 +1288,7 @@
         <v>Silky Anteater</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1">
         <v>2</v>
@@ -1307,7 +1301,7 @@
         <v>Silver Pika</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1">
         <v>2</v>
@@ -1320,7 +1314,7 @@
         <v>Siberian Chipmunk</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1">
         <v>2</v>
@@ -1333,7 +1327,7 @@
         <v>Colo Colo Opossum</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1">
         <v>2</v>
@@ -1346,7 +1340,7 @@
         <v>Pygmy Jerboa</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1">
         <v>2</v>
@@ -1359,7 +1353,7 @@
         <v>Bumblebee Bat</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1">
         <v>2</v>
@@ -1372,7 +1366,7 @@
         <v>Shrew Mole</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1">
         <v>3</v>
@@ -1385,7 +1379,7 @@
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1">
         <v>3</v>
@@ -1398,7 +1392,7 @@
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
         <v>3</v>
@@ -1411,7 +1405,7 @@
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
         <v>3</v>
@@ -1424,7 +1418,7 @@
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
         <v>3</v>
@@ -1437,7 +1431,7 @@
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
         <v>3</v>
@@ -1450,7 +1444,7 @@
         <v>Goanna</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
         <v>3</v>
@@ -1463,7 +1457,7 @@
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1">
         <v>3</v>
@@ -1476,7 +1470,7 @@
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1">
         <v>3</v>
@@ -1489,7 +1483,7 @@
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <v>3</v>
@@ -1502,7 +1496,7 @@
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
         <v>3</v>
@@ -1515,7 +1509,7 @@
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
         <v>3</v>
@@ -1528,7 +1522,7 @@
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
         <v>3</v>
@@ -1541,7 +1535,7 @@
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
         <v>3</v>
@@ -1554,7 +1548,7 @@
         <v>Bee</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
         <v>3</v>
@@ -1567,7 +1561,7 @@
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1">
         <v>3</v>
@@ -1580,7 +1574,7 @@
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1">
         <v>4</v>
@@ -1593,7 +1587,7 @@
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1">
         <v>4</v>
@@ -1606,7 +1600,7 @@
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
         <v>4</v>
@@ -1619,7 +1613,7 @@
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
         <v>4</v>
@@ -1632,7 +1626,7 @@
         <v>Siamang</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1">
         <v>4</v>
@@ -1645,7 +1639,7 @@
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1">
         <v>4</v>
@@ -1658,7 +1652,7 @@
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1">
         <v>4</v>
@@ -1671,7 +1665,7 @@
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1">
         <v>4</v>
@@ -1684,7 +1678,7 @@
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1">
         <v>4</v>
@@ -1697,7 +1691,7 @@
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
         <v>4</v>
@@ -1710,7 +1704,7 @@
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1">
         <v>4</v>
@@ -1723,7 +1717,7 @@
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1">
         <v>4</v>
@@ -1736,7 +1730,7 @@
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1">
         <v>4</v>
@@ -1749,7 +1743,7 @@
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1">
         <v>4</v>
@@ -1762,7 +1756,7 @@
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1">
         <v>4</v>
@@ -1775,7 +1769,7 @@
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1">
         <v>4</v>
@@ -1802,782 +1796,782 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.7109375"/>
-    <col min="3" max="3" customWidth="true" width="25.42578125"/>
-    <col min="15" max="15" customWidth="true" width="23.42578125"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="0">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1" t="str" s="0">
+      <c r="C1" t="str">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str" s="0">
+      <c r="O1" t="str">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>3</v>
       </c>
-      <c r="C3" t="str" s="0">
+      <c r="C3" t="str">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str" s="0">
+      <c r="O3" t="str">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" t="s" s="0">
+      <c r="M4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="C5" t="str" s="0">
+      <c r="C5" t="str">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str" s="0">
+      <c r="O5" t="str">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="0">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="N6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="0">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>7</v>
       </c>
-      <c r="C7" t="str" s="0">
+      <c r="C7" t="str">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str" s="0">
+      <c r="O7" t="str">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="0">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>8</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="F8" t="s">
         <v>4</v>
       </c>
-      <c r="L8" t="s" s="0">
+      <c r="L8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="0">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>9</v>
       </c>
-      <c r="C9" t="str" s="0">
+      <c r="C9" t="str">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str" s="0">
+      <c r="O9" t="str">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="0">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>10</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="N10" t="s" s="0">
+      <c r="N10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="0">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>11</v>
       </c>
-      <c r="C11" t="str" s="0">
+      <c r="C11" t="str">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str" s="0">
+      <c r="O11" t="str">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="0">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="E12" t="s" s="0">
+      <c r="E12" t="s">
         <v>7</v>
       </c>
-      <c r="M12" t="s" s="0">
+      <c r="M12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="0">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>13</v>
       </c>
-      <c r="C13" t="str" s="0">
+      <c r="C13" t="str">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str" s="0">
+      <c r="O13" t="str">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="0">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>14</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="N14" t="s" s="0">
+      <c r="N14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="0">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>15</v>
       </c>
-      <c r="C15" t="str" s="0">
+      <c r="C15" t="str">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str" s="0">
+      <c r="O15" t="str">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="0">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>16</v>
       </c>
-      <c r="G16" t="s" s="0">
+      <c r="G16" t="s">
         <v>4</v>
       </c>
-      <c r="K16" t="s" s="0">
+      <c r="K16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="0">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>17</v>
       </c>
-      <c r="C17" t="str" s="0">
+      <c r="C17" t="str">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str" s="0">
+      <c r="O17" t="str">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="0">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>18</v>
       </c>
-      <c r="D18" t="s" s="0">
+      <c r="D18" t="s">
         <v>8</v>
       </c>
-      <c r="N18" t="s" s="0">
+      <c r="N18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="0">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>19</v>
       </c>
-      <c r="C19" t="str" s="0">
+      <c r="C19" t="str">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str" s="0">
+      <c r="O19" t="str">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="0">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>20</v>
       </c>
-      <c r="E20" t="s" s="0">
+      <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="M20" t="s" s="0">
+      <c r="M20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="0">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>21</v>
       </c>
-      <c r="C21" t="str" s="0">
+      <c r="C21" t="str">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str" s="0">
+      <c r="O21" t="str">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="0">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>22</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="N22" t="s" s="0">
+      <c r="N22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="0">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>23</v>
       </c>
-      <c r="C23" t="str" s="0">
+      <c r="C23" t="str">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str" s="0">
+      <c r="O23" t="str">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="0">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>24</v>
       </c>
-      <c r="F24" t="s" s="0">
+      <c r="F24" t="s">
         <v>11</v>
       </c>
-      <c r="L24" t="s" s="0">
+      <c r="L24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="0">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>25</v>
       </c>
-      <c r="C25" t="str" s="0">
+      <c r="C25" t="str">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str" s="0">
+      <c r="O25" t="str">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="0">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>26</v>
       </c>
-      <c r="D26" t="s" s="0">
+      <c r="D26" t="s">
         <v>10</v>
       </c>
-      <c r="N26" t="s" s="0">
+      <c r="N26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="0">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>27</v>
       </c>
-      <c r="C27" t="str" s="0">
+      <c r="C27" t="str">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str" s="0">
+      <c r="O27" t="str">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="0">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>28</v>
       </c>
-      <c r="E28" t="s" s="0">
+      <c r="E28" t="s">
         <v>11</v>
       </c>
-      <c r="M28" t="s" s="0">
+      <c r="M28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="0">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>29</v>
       </c>
-      <c r="C29" t="str" s="0">
+      <c r="C29" t="str">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str" s="0">
+      <c r="O29" t="str">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="0">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>30</v>
       </c>
-      <c r="D30" t="s" s="0">
+      <c r="D30" t="s">
         <v>11</v>
       </c>
-      <c r="N30" t="s" s="0">
+      <c r="N30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="0">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>31</v>
       </c>
-      <c r="C31" t="str" s="0">
+      <c r="C31" t="str">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str" s="0">
+      <c r="O31" t="str">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="0">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>32</v>
       </c>
-      <c r="H32" t="s" s="0">
+      <c r="H32" t="s">
         <v>13</v>
       </c>
-      <c r="I32" t="s" s="0">
+      <c r="I32" t="s">
         <v>15</v>
       </c>
-      <c r="J32" t="s" s="0">
+      <c r="J32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="0">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>33</v>
       </c>
-      <c r="C33" t="str" s="0">
+      <c r="C33" t="str">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str" s="0">
+      <c r="O33" t="str">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="0">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>34</v>
       </c>
-      <c r="B34" t="str" s="0">
+      <c r="B34" t="str">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s" s="0">
+      <c r="D34" t="s">
         <v>4</v>
       </c>
-      <c r="N34" t="s" s="0">
+      <c r="N34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="0">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>35</v>
       </c>
-      <c r="C35" t="s" s="0">
+      <c r="C35" t="s">
         <v>12</v>
       </c>
-      <c r="O35" t="str" s="0">
+      <c r="O35" t="str">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="0">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>36</v>
       </c>
-      <c r="B36" t="str" s="0">
+      <c r="B36" t="str">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s" s="0">
+      <c r="E36" t="s">
         <v>4</v>
       </c>
-      <c r="M36" t="s" s="0">
+      <c r="M36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="0">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>37</v>
       </c>
-      <c r="C37" t="str" s="0">
+      <c r="C37" t="str">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str" s="0">
+      <c r="O37" t="str">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="0">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>38</v>
       </c>
-      <c r="D38" t="s" s="0">
+      <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="N38" t="s" s="0">
+      <c r="N38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="0">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>39</v>
       </c>
-      <c r="C39" t="str" s="0">
+      <c r="C39" t="str">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str" s="0">
+      <c r="O39" t="str">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="0">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>40</v>
       </c>
-      <c r="F40" t="s" s="0">
+      <c r="F40" t="s">
         <v>4</v>
       </c>
-      <c r="L40" t="s" s="0">
+      <c r="L40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="0">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>41</v>
       </c>
-      <c r="C41" t="str" s="0">
+      <c r="C41" t="str">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str" s="0">
+      <c r="O41" t="str">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="0">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>42</v>
       </c>
-      <c r="D42" t="s" s="0">
+      <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="N42" t="s" s="0">
+      <c r="N42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="0">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>43</v>
       </c>
-      <c r="C43" t="str" s="0">
+      <c r="C43" t="str">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str" s="0">
+      <c r="O43" t="str">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="0">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>44</v>
       </c>
-      <c r="E44" t="s" s="0">
+      <c r="E44" t="s">
         <v>7</v>
       </c>
-      <c r="M44" t="s" s="0">
+      <c r="M44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="0">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>45</v>
       </c>
-      <c r="C45" t="str" s="0">
+      <c r="C45" t="str">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str" s="0">
+      <c r="O45" t="str">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="0">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>46</v>
       </c>
-      <c r="D46" t="s" s="0">
+      <c r="D46" t="s">
         <v>7</v>
       </c>
-      <c r="N46" t="s" s="0">
+      <c r="N46" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="0">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>47</v>
       </c>
-      <c r="C47" t="str" s="0">
+      <c r="C47" t="str">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str" s="0">
+      <c r="O47" t="str">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="0">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>48</v>
       </c>
-      <c r="G48" t="s" s="0">
+      <c r="G48" t="s">
         <v>4</v>
       </c>
-      <c r="K48" t="s" s="0">
+      <c r="K48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="0">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>49</v>
       </c>
-      <c r="C49" t="str" s="0">
+      <c r="C49" t="str">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str" s="0">
+      <c r="O49" t="str">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="0">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>50</v>
       </c>
-      <c r="D50" t="s" s="0">
+      <c r="D50" t="s">
         <v>8</v>
       </c>
-      <c r="N50" t="s" s="0">
+      <c r="N50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="0">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>51</v>
       </c>
-      <c r="C51" t="str" s="0">
+      <c r="C51" t="str">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str" s="0">
+      <c r="O51" t="str">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="0">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>52</v>
       </c>
-      <c r="E52" t="s" s="0">
+      <c r="E52" t="s">
         <v>9</v>
       </c>
-      <c r="M52" t="s" s="0">
+      <c r="M52" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="0">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>53</v>
       </c>
-      <c r="C53" t="str" s="0">
+      <c r="C53" t="str">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str" s="0">
+      <c r="O53" t="str">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="0">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>54</v>
       </c>
-      <c r="D54" t="s" s="0">
+      <c r="D54" t="s">
         <v>9</v>
       </c>
-      <c r="N54" t="s" s="0">
+      <c r="N54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="0">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>55</v>
       </c>
-      <c r="C55" t="str" s="0">
+      <c r="C55" t="str">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str" s="0">
+      <c r="O55" t="str">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="0">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>56</v>
       </c>
-      <c r="F56" t="s" s="0">
+      <c r="F56" t="s">
         <v>11</v>
       </c>
-      <c r="L56" t="s" s="0">
+      <c r="L56" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="0">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>57</v>
       </c>
-      <c r="C57" t="str" s="0">
+      <c r="C57" t="str">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str" s="0">
+      <c r="O57" t="str">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="0">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>58</v>
       </c>
-      <c r="D58" t="s" s="0">
+      <c r="D58" t="s">
         <v>10</v>
       </c>
-      <c r="N58" t="s" s="0">
+      <c r="N58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="0">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>59</v>
       </c>
-      <c r="C59" t="str" s="0">
+      <c r="C59" t="str">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str" s="0">
+      <c r="O59" t="str">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="0">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>60</v>
       </c>
-      <c r="E60" t="s" s="0">
+      <c r="E60" t="s">
         <v>11</v>
       </c>
-      <c r="M60" t="s" s="0">
+      <c r="M60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="0">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>61</v>
       </c>
-      <c r="C61" t="str" s="0">
+      <c r="C61" t="str">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str" s="0">
+      <c r="O61" t="str">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="0">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>62</v>
       </c>
-      <c r="D62" t="s" s="0">
+      <c r="D62" t="s">
         <v>11</v>
       </c>
-      <c r="N62" t="s" s="0">
+      <c r="N62" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="0">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>63</v>
       </c>
-      <c r="C63" t="str" s="0">
+      <c r="C63" t="str">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str" s="0">
+      <c r="O63" t="str">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:O64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:O64">
     <sortCondition ref="A1:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2588,782 +2582,779 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD84F6-D856-4FCA-9254-65D9DBB06268}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="56" zoomScaleNormal="39" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.7109375"/>
-    <col min="3" max="3" customWidth="true" width="25.42578125"/>
-    <col min="4" max="4" customWidth="true" width="25.7109375"/>
-    <col min="14" max="14" customWidth="true" width="23.28515625"/>
-    <col min="15" max="15" customWidth="true" width="23.42578125"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="15" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="0">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="C1" t="str" s="0">
+      <c r="C1" t="str">
         <f>Helper!D2</f>
         <v>Okapi</v>
       </c>
-      <c r="O1" t="str" s="0">
+      <c r="O1" t="str">
         <f>Helper!D35</f>
         <v>Golden Eagle</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s" s="0">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" t="str" s="0">
+      <c r="C3" t="str">
         <f>Helper!D17</f>
         <v>Four-Striped Grass Mouse</v>
       </c>
-      <c r="O3" t="str" s="0">
+      <c r="O3" t="str">
         <f>Helper!D50</f>
         <v>Spongilla Fly</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="0">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="M4" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" t="str" s="0">
+      <c r="C5" t="str">
         <f>Helper!D9</f>
         <v>Striped Polecat</v>
       </c>
-      <c r="O5" t="str" s="0">
+      <c r="O5" t="str">
         <f>Helper!D42</f>
         <v>Veined Octopus</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="0">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="D6" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="0">
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="C7" t="str" s="0">
+      <c r="C7" t="str">
         <f>Helper!D10</f>
         <v>Giant striped mongoose</v>
       </c>
-      <c r="O7" t="str" s="0">
+      <c r="O7" t="str">
         <f>Helper!D43</f>
         <v>Puffer Fish</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="0">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="F8" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="0">
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="C9" t="str" s="0">
+      <c r="C9" t="str">
         <f>Helper!D6</f>
         <v>Side-striped jackal</v>
       </c>
-      <c r="O9" t="str" s="0">
+      <c r="O9" t="str">
         <f>Helper!D39</f>
         <v>Palaeocastor</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="0">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="N10" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="0">
+      <c r="N10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C11" t="str" s="0">
+      <c r="C11" t="str">
         <f>Helper!D13</f>
         <v>Striped Possum</v>
       </c>
-      <c r="O11" t="str" s="0">
+      <c r="O11" t="str">
         <f>Helper!D46</f>
         <v>Trapdoor Spider</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="0">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="E12" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="M12" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="0">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="C13" t="str" s="0">
+      <c r="C13" t="str">
         <f>Helper!D5</f>
         <v>Striped dolphin</v>
       </c>
-      <c r="O13" t="str" s="0">
+      <c r="O13" t="str">
         <f>Helper!D38</f>
         <v>Lungfish</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="0">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="D14" t="s" s="0">
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="N14" t="s" s="0">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="0">
+      <c r="N14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="C15" t="str" s="0">
+      <c r="C15" t="str">
         <f>Helper!D14</f>
         <v>Chequered elephant shrew</v>
       </c>
-      <c r="O15" t="str" s="0">
+      <c r="O15" t="str">
         <f>Helper!D47</f>
         <v>Tent-making Bat</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="0">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="G16" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="K16" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="0">
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="C17" t="str" s="0">
+      <c r="C17" t="str">
         <f>Helper!D7</f>
         <v>Wildcat</v>
       </c>
-      <c r="O17" t="str" s="0">
+      <c r="O17" t="str">
         <f>Helper!D40</f>
         <v>Goanna</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="0">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="D18" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="N18" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="0">
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="C19" t="str" s="0">
+      <c r="C19" t="str">
         <f>Helper!D12</f>
         <v>Highland Streaked Tenrec</v>
       </c>
-      <c r="O19" t="str" s="0">
+      <c r="O19" t="str">
         <f>Helper!D45</f>
         <v>Rufous Hornero</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="0">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="E20" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="M20" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="0">
+      <c r="E20" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="str" s="0">
+      <c r="M20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
         <f>Helper!D4</f>
         <v>Striped hyena</v>
       </c>
-      <c r="O21" t="str" s="0">
+      <c r="O21" t="str">
         <f>Helper!D37</f>
         <v>Homo habilis</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="0">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="D22" t="s" s="0">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="N22" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="0">
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="C23" t="str" s="0">
+      <c r="C23" t="str">
         <f>Helper!D15</f>
         <v>Fire-footed Rope Squirrel</v>
       </c>
-      <c r="O23" t="str" s="0">
+      <c r="O23" t="str">
         <f>Helper!D48</f>
         <v>Bee</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="0">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="F24" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="L24" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="0">
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="C25" t="str" s="0">
+      <c r="C25" t="str">
         <f>Helper!D8</f>
         <v>Striped Rabbit</v>
       </c>
-      <c r="O25" t="str" s="0">
+      <c r="O25" t="str">
         <f>Helper!D41</f>
         <v>Montezuma Oropendola</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="0">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="D26" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="N26" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="0">
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="C27" t="str" s="0">
+      <c r="C27" t="str">
         <f>Helper!D11</f>
         <v>Numbat</v>
       </c>
-      <c r="O27" t="str" s="0">
+      <c r="O27" t="str">
         <f>Helper!D44</f>
         <v>New Caledonian Crow</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="0">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="E28" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="M28" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="0">
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="C29" t="str" s="0">
+      <c r="C29" t="str">
         <f>Helper!D3</f>
         <v>Kudu</v>
       </c>
-      <c r="O29" t="str" s="0">
+      <c r="O29" t="str">
         <f>Helper!D36</f>
         <v>Cathedral Termite</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="0">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="D30" t="s" s="0">
+      <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="N30" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="0">
+      <c r="N30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="C31" t="str" s="0">
+      <c r="C31" t="str">
         <f>Helper!D16</f>
         <v>Badger Bat</v>
       </c>
-      <c r="O31" t="str" s="0">
+      <c r="O31" t="str">
         <f>Helper!D49</f>
         <v>Dung Beetle</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="0">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="H32" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="I32" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="J32" t="s" s="0">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="0">
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="C33" t="str" s="0">
+      <c r="C33" t="str">
         <f>Helper!D18</f>
         <v>Sea Otter</v>
       </c>
-      <c r="O33" t="str" s="0">
+      <c r="O33" t="str">
         <f>Helper!D51</f>
         <v>Emperor Penguin</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="0">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="str" s="0">
+      <c r="B34" t="str">
         <f>Helper!A2</f>
         <v>Bumblebee Bat</v>
       </c>
-      <c r="D34" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="N34" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="0">
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="C35" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="O35" t="str" s="0">
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="O35" t="str">
         <f>Helper!D66</f>
         <v>Lined Seahorse</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="0">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="str" s="0">
+      <c r="B36" t="str">
         <f>Helper!A3</f>
         <v>Shrew Mole</v>
       </c>
-      <c r="E36" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="M36" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="0">
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="C37" t="str" s="0">
+      <c r="C37" t="str">
         <f>Helper!D25</f>
         <v>Southern Ningaui</v>
       </c>
-      <c r="O37" t="str" s="0">
+      <c r="O37" t="str">
         <f>Helper!D58</f>
         <v>Owl Monkey</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="0">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="D38" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="N38" t="s" s="0">
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="0">
-        <v>38</v>
-      </c>
-      <c r="C39" t="str" s="0">
+      <c r="C39" t="str">
         <f>Helper!D26</f>
         <v>Grasshopper Mouse</v>
       </c>
-      <c r="O39" t="str" s="0">
+      <c r="O39" t="str">
         <f>Helper!D59</f>
         <v>Caspian Terns</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="0">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="F40" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="L40" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="0">
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="C41" t="str" s="0">
+      <c r="C41" t="str">
         <f>Helper!D22</f>
         <v>Sibree Dwarf Lemur</v>
       </c>
-      <c r="O41" t="str" s="0">
+      <c r="O41" t="str">
         <f>Helper!D55</f>
         <v>Pacific Spiny Lumpsucker</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="0">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="D42" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="N42" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="0">
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="C43" t="str" s="0">
+      <c r="C43" t="str">
         <f>Helper!D29</f>
         <v>Silver Pika</v>
       </c>
-      <c r="O43" t="str" s="0">
+      <c r="O43" t="str">
         <f>Helper!D62</f>
         <v>Peacock Wrasse</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="0">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="E44" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="M44" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="0">
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="M44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="C45" t="str" s="0">
+      <c r="C45" t="str">
         <f>Helper!D21</f>
         <v>Mara</v>
       </c>
-      <c r="O45" t="str" s="0">
+      <c r="O45" t="str">
         <f>Helper!D54</f>
         <v>Siamang</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="0">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="D46" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="N46" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="0">
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="N46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="C47" t="str" s="0">
+      <c r="C47" t="str">
         <f>Helper!D30</f>
         <v>Siberian Chipmunk</v>
       </c>
-      <c r="O47" t="str" s="0">
+      <c r="O47" t="str">
         <f>Helper!D63</f>
         <v>Darwin's Frogs</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="0">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="G48" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="K48" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="0">
+      <c r="G48" t="s">
+        <v>34</v>
+      </c>
+      <c r="K48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="C49" t="str" s="0">
+      <c r="C49" t="str">
         <f>Helper!D23</f>
         <v>Itjaritjari</v>
       </c>
-      <c r="O49" t="str" s="0">
+      <c r="O49" t="str">
         <f>Helper!D56</f>
         <v>Bat-Eared Fox</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="0">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="D50" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="N50" t="s" s="0">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="0">
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="N50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="C51" t="str" s="0">
+      <c r="C51" t="str">
         <f>Helper!D28</f>
         <v>Silky Anteater</v>
       </c>
-      <c r="O51" t="str" s="0">
+      <c r="O51" t="str">
         <f>Helper!D61</f>
         <v>Spotted sandpiper</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="0">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>51</v>
       </c>
-      <c r="E52" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="M52" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="0">
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="M52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>52</v>
       </c>
-      <c r="C53" t="str" s="0">
+      <c r="C53" t="str">
         <f>Helper!D20</f>
         <v>Dik Dik</v>
       </c>
-      <c r="O53" t="str" s="0">
+      <c r="O53" t="str">
         <f>Helper!D53</f>
         <v>Wolverine</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="0">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>53</v>
       </c>
-      <c r="D54" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="N54" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="0">
+      <c r="D54" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>54</v>
       </c>
-      <c r="C55" t="str" s="0">
+      <c r="C55" t="str">
         <f>Helper!D31</f>
         <v>Colo Colo Opossum</v>
       </c>
-      <c r="O55" t="str" s="0">
+      <c r="O55" t="str">
         <f>Helper!D64</f>
         <v>Giant Water Bug</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="0">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>55</v>
       </c>
-      <c r="F56" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="L56" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="0">
+      <c r="F56" t="s">
+        <v>34</v>
+      </c>
+      <c r="L56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>56</v>
       </c>
-      <c r="C57" t="str" s="0">
+      <c r="C57" t="str">
         <f>Helper!D24</f>
         <v>Bulldog Bat</v>
       </c>
-      <c r="O57" t="str" s="0">
+      <c r="O57" t="str">
         <f>Helper!D57</f>
         <v>Greater Flamingo</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="0">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>57</v>
       </c>
-      <c r="D58" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="N58" t="s" s="0">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="0">
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+      <c r="N58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>58</v>
       </c>
-      <c r="C59" t="str" s="0">
+      <c r="C59" t="str">
         <f>Helper!D27</f>
         <v>Thor's Hero Shrew</v>
       </c>
-      <c r="O59" t="str" s="0">
+      <c r="O59" t="str">
         <f>Helper!D60</f>
         <v>Dyak Fruit Bat</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="0">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>59</v>
       </c>
-      <c r="E60" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="M60" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="0">
+      <c r="E60" t="s">
+        <v>23</v>
+      </c>
+      <c r="M60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="C61" t="str" s="0">
+      <c r="C61" t="str">
         <f>Helper!D19</f>
         <v xml:space="preserve">Rock Hyrax </v>
       </c>
-      <c r="O61" t="str" s="0">
+      <c r="O61" t="str">
         <f>Helper!D52</f>
         <v>Greater Rhea</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="0">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>61</v>
       </c>
-      <c r="D62" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="N62" t="s" s="0">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="0">
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>62</v>
       </c>
-      <c r="C63" t="str" s="0">
+      <c r="C63" t="str">
         <f>Helper!D32</f>
         <v>Pygmy Jerboa</v>
       </c>
-      <c r="O63" t="str" s="0">
+      <c r="O63" t="str">
         <f>Helper!D65</f>
         <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
@@ -3376,50 +3367,779 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="D2:D30"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D2" t="s" s="0">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="C1" t="str">
+        <f>Helper!D2</f>
+        <v>Okapi</v>
+      </c>
+      <c r="O1" t="str">
+        <f>Helper!D35</f>
+        <v>Golden Eagle</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="s" s="0">
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Helper!D17</f>
+        <v>Four-Striped Grass Mouse</v>
+      </c>
+      <c r="O3" t="str">
+        <f>Helper!D50</f>
+        <v>Spongilla Fly</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Helper!D9</f>
+        <v>Striped Polecat</v>
+      </c>
+      <c r="O5" t="str">
+        <f>Helper!D42</f>
+        <v>Veined Octopus</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Helper!D10</f>
+        <v>Giant striped mongoose</v>
+      </c>
+      <c r="O7" t="str">
+        <f>Helper!D43</f>
+        <v>Puffer Fish</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Helper!D6</f>
+        <v>Side-striped jackal</v>
+      </c>
+      <c r="O9" t="str">
+        <f>Helper!D39</f>
+        <v>Palaeocastor</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Helper!D13</f>
+        <v>Striped Possum</v>
+      </c>
+      <c r="O11" t="str">
+        <f>Helper!D46</f>
+        <v>Trapdoor Spider</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Helper!D5</f>
+        <v>Striped dolphin</v>
+      </c>
+      <c r="O13" t="str">
+        <f>Helper!D38</f>
+        <v>Lungfish</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Helper!D14</f>
+        <v>Chequered elephant shrew</v>
+      </c>
+      <c r="O15" t="str">
+        <f>Helper!D47</f>
+        <v>Tent-making Bat</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Helper!D7</f>
+        <v>Wildcat</v>
+      </c>
+      <c r="O17" t="str">
+        <f>Helper!D40</f>
+        <v>Goanna</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Helper!D12</f>
+        <v>Highland Streaked Tenrec</v>
+      </c>
+      <c r="O19" t="str">
+        <f>Helper!D45</f>
+        <v>Rufous Hornero</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Helper!D4</f>
+        <v>Striped hyena</v>
+      </c>
+      <c r="O21" t="str">
+        <f>Helper!D37</f>
+        <v>Homo habilis</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D10" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s" s="0">
+      <c r="C23" t="str">
+        <f>Helper!D15</f>
+        <v>Fire-footed Rope Squirrel</v>
+      </c>
+      <c r="O23" t="str">
+        <f>Helper!D48</f>
+        <v>Bee</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s" s="0">
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="str">
+        <f>Helper!D8</f>
+        <v>Striped Rabbit</v>
+      </c>
+      <c r="O25" t="str">
+        <f>Helper!D41</f>
+        <v>Montezuma Oropendola</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Helper!D11</f>
+        <v>Numbat</v>
+      </c>
+      <c r="O27" t="str">
+        <f>Helper!D44</f>
+        <v>New Caledonian Crow</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="str">
+        <f>Helper!D3</f>
+        <v>Kudu</v>
+      </c>
+      <c r="O29" t="str">
+        <f>Helper!D36</f>
+        <v>Cathedral Termite</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
         <v>21</v>
+      </c>
+      <c r="N30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="str">
+        <f>Helper!D16</f>
+        <v>Badger Bat</v>
+      </c>
+      <c r="O31" t="str">
+        <f>Helper!D49</f>
+        <v>Dung Beetle</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="str">
+        <f>Helper!D18</f>
+        <v>Sea Otter</v>
+      </c>
+      <c r="O33" t="str">
+        <f>Helper!D51</f>
+        <v>Emperor Penguin</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="str">
+        <f>Helper!A2</f>
+        <v>Bumblebee Bat</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="N34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O35" t="str">
+        <f>Helper!D66</f>
+        <v>Lined Seahorse</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="str">
+        <f>Helper!A3</f>
+        <v>Shrew Mole</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="str">
+        <f>Helper!D25</f>
+        <v>Southern Ningaui</v>
+      </c>
+      <c r="O37" t="str">
+        <f>Helper!D58</f>
+        <v>Owl Monkey</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="str">
+        <f>Helper!D26</f>
+        <v>Grasshopper Mouse</v>
+      </c>
+      <c r="O39" t="str">
+        <f>Helper!D59</f>
+        <v>Caspian Terns</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="str">
+        <f>Helper!D22</f>
+        <v>Sibree Dwarf Lemur</v>
+      </c>
+      <c r="O41" t="str">
+        <f>Helper!D55</f>
+        <v>Pacific Spiny Lumpsucker</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="str">
+        <f>Helper!D29</f>
+        <v>Silver Pika</v>
+      </c>
+      <c r="O43" t="str">
+        <f>Helper!D62</f>
+        <v>Peacock Wrasse</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+      <c r="M44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="str">
+        <f>Helper!D21</f>
+        <v>Mara</v>
+      </c>
+      <c r="O45" t="str">
+        <f>Helper!D54</f>
+        <v>Siamang</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="N46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="str">
+        <f>Helper!D30</f>
+        <v>Siberian Chipmunk</v>
+      </c>
+      <c r="O47" t="str">
+        <f>Helper!D63</f>
+        <v>Darwin's Frogs</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s">
+        <v>34</v>
+      </c>
+      <c r="K48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="str">
+        <f>Helper!D23</f>
+        <v>Itjaritjari</v>
+      </c>
+      <c r="O49" t="str">
+        <f>Helper!D56</f>
+        <v>Bat-Eared Fox</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>45</v>
+      </c>
+      <c r="N50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="str">
+        <f>Helper!D28</f>
+        <v>Silky Anteater</v>
+      </c>
+      <c r="O51" t="str">
+        <f>Helper!D61</f>
+        <v>Spotted sandpiper</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="E52" t="s">
+        <v>34</v>
+      </c>
+      <c r="M52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="str">
+        <f>Helper!D20</f>
+        <v>Dik Dik</v>
+      </c>
+      <c r="O53" t="str">
+        <f>Helper!D53</f>
+        <v>Wolverine</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="D54" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="C55" t="str">
+        <f>Helper!D31</f>
+        <v>Colo Colo Opossum</v>
+      </c>
+      <c r="O55" t="str">
+        <f>Helper!D64</f>
+        <v>Giant Water Bug</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="F56" t="s">
+        <v>34</v>
+      </c>
+      <c r="L56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="C57" t="str">
+        <f>Helper!D24</f>
+        <v>Bulldog Bat</v>
+      </c>
+      <c r="O57" t="str">
+        <f>Helper!D57</f>
+        <v>Greater Flamingo</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="N58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="C59" t="str">
+        <f>Helper!D27</f>
+        <v>Thor's Hero Shrew</v>
+      </c>
+      <c r="O59" t="str">
+        <f>Helper!D60</f>
+        <v>Dyak Fruit Bat</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="E60" t="s">
+        <v>38</v>
+      </c>
+      <c r="M60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="str">
+        <f>Helper!D19</f>
+        <v xml:space="preserve">Rock Hyrax </v>
+      </c>
+      <c r="O61" t="str">
+        <f>Helper!D52</f>
+        <v>Greater Rhea</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="C63" t="str">
+        <f>Helper!D32</f>
+        <v>Pygmy Jerboa</v>
+      </c>
+      <c r="O63" t="str">
+        <f>Helper!D65</f>
+        <v xml:space="preserve">Three-Spined stickleback </v>
       </c>
     </row>
   </sheetData>

</xml_diff>